<commit_message>
minor updates to abstract assignments and views.  add method to import abstract data from excel.
</commit_message>
<xml_diff>
--- a/app/assets/images/abstract_assignments.xlsx
+++ b/app/assets/images/abstract_assignments.xlsx
@@ -1,20 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="27795" windowHeight="13605"/>
+    <workbookView xWindow="9180" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725" iterateDelta="1E-4"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="780" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="776" uniqueCount="538">
   <si>
     <t>First Author's last name</t>
   </si>
@@ -310,9 +315,6 @@
     <t>Cell Encapsulation in Complex 3D Hydrogel Microstructures via Dynamic Stereolithography</t>
   </si>
   <si>
-    <t>LCD</t>
-  </si>
-  <si>
     <t>Coskun</t>
   </si>
   <si>
@@ -616,9 +618,6 @@
     <t>Hur</t>
   </si>
   <si>
-    <t>Sung Sik Hur</t>
-  </si>
-  <si>
     <t>3D Intracellular and Traction Forces of Vascular Endothelial Cells</t>
   </si>
   <si>
@@ -1291,15 +1290,6 @@
     <t>Oral Session I</t>
   </si>
   <si>
-    <t>Seitzer</t>
-  </si>
-  <si>
-    <t>Seitzer, Phillip M*† and Facciotti, Marc T.*†</t>
-  </si>
-  <si>
-    <t>A software platform for linking genotype to phenotype in closely related microbial species through genomic context comparison</t>
-  </si>
-  <si>
     <t>Seker</t>
   </si>
   <si>
@@ -1619,13 +1609,37 @@
   </si>
   <si>
     <t>Characterization of Intracellular Streaming and Traction Forces in Migrating Physarum Plasmodia</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> N/A</t>
+  </si>
+  <si>
+    <t>Sung Sik Hur, Juan Carlos del Álamo, Sung-Hwan Min, Edward Vuong, Young Min Paik, McKenna Geary, Kuei-Chun Wang, Yi-Ting Yeh, Yi-Shuan Li, Juan Lasheras, Shu Chien</t>
+  </si>
+  <si>
+    <t>LCD 1</t>
+  </si>
+  <si>
+    <t>LCD 2</t>
+  </si>
+  <si>
+    <t>LCD 3</t>
+  </si>
+  <si>
+    <t>LCD 4</t>
+  </si>
+  <si>
+    <t>Making Heparin Gel Sandwiches with Liver Cells</t>
+  </si>
+  <si>
+    <t>Elena Foster, Jungmok You, Alexander Revzin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1639,6 +1653,33 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1658,10 +1699,70 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1688,9 +1789,70 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="61">
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="27" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="29" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="31" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="33" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="35" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="37" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="39" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="12" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="14" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="16" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="18" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="20" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="22" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="24" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="28" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="30" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="32" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="34" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="36" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="38" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="40" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1982,23 +2144,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AMK175"/>
+  <dimension ref="A1:AMI175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52.28515625" style="3" customWidth="1"/>
     <col min="3" max="3" width="45.140625" style="3" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="6" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="1025" width="9.140625" style="5"/>
+    <col min="6" max="1023" width="8.85546875" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1025" s="4" customFormat="1" ht="30">
+    <row r="1" spans="1:1023" s="4" customFormat="1" ht="30">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3032,52 +3194,50 @@
       <c r="AMG1" s="3"/>
       <c r="AMH1" s="3"/>
       <c r="AMI1" s="3"/>
-      <c r="AMJ1" s="3"/>
-      <c r="AMK1" s="3"/>
-    </row>
-    <row r="2" spans="1:1025" ht="45">
+    </row>
+    <row r="2" spans="1:1023" ht="60">
       <c r="A2" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>6</v>
+        <v>13</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>14</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1025" ht="45">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1023" ht="45">
       <c r="A3" s="5" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
+        <v>41</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1025" ht="60">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1023" ht="45">
       <c r="A4" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>14</v>
+        <v>304</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>305</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>15</v>
+        <v>306</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>8</v>
@@ -3086,406 +3246,406 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:1025" ht="45">
-      <c r="A5" t="s">
-        <v>13</v>
+    <row r="5" spans="1:1023" ht="45">
+      <c r="A5" s="5" t="s">
+        <v>398</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>399</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="6">
-        <v>1</v>
+        <v>400</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1025" ht="30">
-      <c r="A6" s="5" t="s">
-        <v>20</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1023" ht="30">
+      <c r="A6" t="s">
+        <v>77</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>22</v>
+        <v>79</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1025" ht="45">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1023" ht="30">
       <c r="A7" s="5" t="s">
-        <v>24</v>
+        <v>228</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>25</v>
+        <v>229</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>26</v>
+        <v>230</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1025" ht="30">
+      <c r="E7" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1023" ht="30">
       <c r="A8" s="5" t="s">
-        <v>28</v>
+        <v>257</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>29</v>
+        <v>258</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
+        <v>259</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1025" ht="60">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1023" ht="30">
       <c r="A9" s="5" t="s">
-        <v>32</v>
+        <v>512</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>33</v>
+        <v>513</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="6">
-        <v>2</v>
+        <v>514</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1025" ht="60">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1023" ht="45">
       <c r="A10" s="5" t="s">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1025" ht="45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1023" ht="30">
       <c r="A11" s="5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1025" ht="45">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1023" ht="45">
       <c r="A12" s="5" t="s">
-        <v>42</v>
+        <v>251</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>43</v>
+        <v>252</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="6">
-        <v>2</v>
+        <v>253</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1025" ht="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1023" ht="60">
       <c r="A13" s="5" t="s">
-        <v>45</v>
+        <v>336</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>46</v>
+        <v>337</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="6">
-        <v>3</v>
+        <v>338</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1025" ht="30">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1023" ht="30">
       <c r="A14" s="5" t="s">
-        <v>48</v>
+        <v>126</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>49</v>
+        <v>127</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>50</v>
+        <v>128</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1025" ht="45">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1023" ht="30">
       <c r="A15" s="5" t="s">
-        <v>51</v>
+        <v>275</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>52</v>
+        <v>276</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>53</v>
+        <v>277</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1025" ht="30">
+      <c r="E15" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1023" ht="45">
       <c r="A16" s="5" t="s">
-        <v>54</v>
+        <v>324</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>55</v>
+        <v>325</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="6">
-        <v>4</v>
+        <v>326</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>31</v>
+        <v>129</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30">
       <c r="A17" s="5" t="s">
-        <v>57</v>
+        <v>455</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>58</v>
+        <v>456</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>59</v>
+        <v>457</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>60</v>
+        <v>129</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="60">
       <c r="A18" s="5" t="s">
-        <v>61</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="D18" s="6">
-        <v>1</v>
+        <v>37</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E18" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="60">
       <c r="A19" s="5" t="s">
-        <v>65</v>
+        <v>134</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D19" s="6">
-        <v>2</v>
+        <v>136</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="45">
       <c r="A20" s="5" t="s">
-        <v>68</v>
+        <v>163</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>69</v>
+        <v>164</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="D20" s="6">
-        <v>3</v>
+        <v>165</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="45">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30">
       <c r="A21" s="5" t="s">
-        <v>71</v>
+        <v>503</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>72</v>
+        <v>504</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D21" s="6">
-        <v>5</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>31</v>
+        <v>505</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="45">
       <c r="A22" s="5" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>75</v>
+        <v>87</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="6">
-        <v>2</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30">
-      <c r="A23" t="s">
-        <v>77</v>
+        <v>88</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="45">
+      <c r="A23" s="5" t="s">
+        <v>200</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>78</v>
+        <v>201</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>79</v>
+        <v>202</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" ht="60">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30">
       <c r="A24" s="5" t="s">
-        <v>81</v>
+        <v>263</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>82</v>
+        <v>264</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D24" s="6">
-        <v>6</v>
+        <v>265</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E24" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="30">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="45">
       <c r="A25" s="5" t="s">
-        <v>81</v>
+        <v>479</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>84</v>
+        <v>480</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D25" s="6">
-        <v>7</v>
+        <v>481</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E25" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="45">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="30">
       <c r="A26" s="5" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D26" s="6">
-        <v>3</v>
+        <v>93</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="45">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="60">
       <c r="A27" s="5" t="s">
-        <v>86</v>
+        <v>295</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>89</v>
+        <v>296</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" s="6">
-        <v>3</v>
+        <v>297</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="45">
       <c r="A28" s="5" t="s">
-        <v>91</v>
+        <v>339</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>92</v>
+        <v>340</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>93</v>
+        <v>341</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>8</v>
@@ -3494,579 +3654,579 @@
         <v>94</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="30">
+    <row r="29" spans="1:5" ht="45">
       <c r="A29" s="5" t="s">
-        <v>95</v>
+        <v>443</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>96</v>
+        <v>444</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="30">
+        <v>445</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="45">
       <c r="A30" s="5" t="s">
-        <v>99</v>
+        <v>160</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>100</v>
+        <v>161</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>101</v>
+        <v>162</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E30" s="7" t="s">
-        <v>102</v>
+      <c r="E30" s="6" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="30">
       <c r="A31" s="5" t="s">
-        <v>103</v>
+        <v>419</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>104</v>
+        <v>420</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D31" s="6">
-        <v>4</v>
+        <v>421</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>12</v>
+        <v>422</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="45">
-      <c r="A32" t="s">
-        <v>106</v>
+      <c r="A32" s="5" t="s">
+        <v>485</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>107</v>
+        <v>486</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D32" s="6">
-        <v>5</v>
+        <v>487</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="30">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="60">
       <c r="A33" s="5" t="s">
-        <v>109</v>
+        <v>248</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>110</v>
+        <v>249</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>111</v>
+        <v>250</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="7" t="s">
-        <v>60</v>
+      <c r="E33" s="9" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="30">
       <c r="A34" s="5" t="s">
-        <v>112</v>
+        <v>57</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D34" s="6">
+        <v>59</v>
+      </c>
+      <c r="D34" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30">
       <c r="A35" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D35" s="6">
-        <v>4</v>
+        <v>110</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>19</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30">
-      <c r="A36" t="s">
-        <v>118</v>
+      <c r="A36" s="5" t="s">
+        <v>141</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="D36" s="6">
-        <v>6</v>
+        <v>143</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="45">
-      <c r="A37" t="s">
-        <v>121</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D37" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="45">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="30">
       <c r="A38" s="5" t="s">
-        <v>124</v>
+        <v>20</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>125</v>
+        <v>21</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="D38" s="6">
-        <v>7</v>
+        <v>22</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E38" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" ht="30">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="45">
       <c r="A39" s="5" t="s">
-        <v>127</v>
+        <v>183</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>128</v>
+        <v>184</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>129</v>
+        <v>185</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E39" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="75">
       <c r="A40" s="5" t="s">
-        <v>131</v>
+        <v>342</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>132</v>
+        <v>343</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>133</v>
+        <v>344</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E40" s="7" t="s">
-        <v>134</v>
+        <v>23</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="60">
       <c r="A41" s="5" t="s">
-        <v>135</v>
+        <v>440</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>136</v>
+        <v>441</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>137</v>
+        <v>442</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="60">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="45">
       <c r="A42" s="5" t="s">
-        <v>138</v>
+        <v>24</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>139</v>
+        <v>25</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>140</v>
+        <v>26</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E42" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="30">
+      <c r="E42" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="45">
       <c r="A43" s="5" t="s">
-        <v>142</v>
+        <v>51</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>143</v>
+        <v>52</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>144</v>
+        <v>53</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E43" s="7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="60">
-      <c r="A44" s="5" t="s">
-        <v>145</v>
+      <c r="E43" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="45">
+      <c r="A44" t="s">
+        <v>216</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>146</v>
+        <v>217</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="D44" s="6">
+        <v>218</v>
+      </c>
+      <c r="D44" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="30">
+      <c r="E44" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="45">
       <c r="A45" s="5" t="s">
-        <v>148</v>
+        <v>254</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>149</v>
+        <v>255</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="D45" s="6">
-        <v>9</v>
-      </c>
-      <c r="E45" s="7" t="s">
-        <v>31</v>
+        <v>256</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="30">
-      <c r="A46" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>153</v>
+      <c r="A46" t="s">
+        <v>407</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>409</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>530</v>
+      </c>
+      <c r="E46" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="60">
+      <c r="A47" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D47" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="45">
-      <c r="A47" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="D47" s="6">
-        <v>5</v>
-      </c>
       <c r="E47" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="30">
       <c r="A48" s="5" t="s">
-        <v>158</v>
+        <v>298</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>159</v>
+        <v>299</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="D48" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E48" s="8" t="s">
-        <v>12</v>
+        <v>300</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="45">
       <c r="A49" s="5" t="s">
-        <v>161</v>
+        <v>309</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>162</v>
+        <v>310</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="D49" s="6">
-        <v>9</v>
+        <v>311</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E49" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="45">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="30">
       <c r="A50" s="5" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E50" s="7" t="s">
-        <v>38</v>
+        <v>101</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="30">
       <c r="A51" s="5" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="D51" s="6">
-        <v>10</v>
+        <v>179</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E51" s="7" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:5" ht="45">
       <c r="A52" s="5" t="s">
-        <v>170</v>
+        <v>366</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>171</v>
+        <v>367</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="D52" s="6">
-        <v>6</v>
+        <v>368</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E52" s="7" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="45">
       <c r="A53" s="5" t="s">
-        <v>173</v>
+        <v>458</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>174</v>
+        <v>459</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>175</v>
+        <v>460</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="30">
+      <c r="E53" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="45">
       <c r="A54" s="5" t="s">
-        <v>173</v>
+        <v>130</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>176</v>
+        <v>131</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="D54" s="6">
-        <v>4</v>
+        <v>132</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="E54" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="30">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="60">
       <c r="A55" s="5" t="s">
-        <v>178</v>
+        <v>354</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>179</v>
+        <v>355</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>180</v>
+        <v>356</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E55" s="7" t="s">
-        <v>102</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:5" ht="30">
       <c r="A56" s="5" t="s">
-        <v>181</v>
+        <v>467</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>182</v>
+        <v>468</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="D56" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E56" s="8" t="s">
-        <v>64</v>
+        <v>469</v>
+      </c>
+      <c r="D56" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>133</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="45">
       <c r="A57" s="5" t="s">
-        <v>184</v>
+        <v>518</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>185</v>
+        <v>519</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>186</v>
+        <v>520</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>8</v>
       </c>
       <c r="E57" s="7" t="s">
-        <v>23</v>
+        <v>133</v>
       </c>
     </row>
     <row r="58" spans="1:5" ht="30">
       <c r="A58" s="5" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="D58" s="6">
-        <v>11</v>
-      </c>
-      <c r="E58" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" ht="30">
+        <v>152</v>
+      </c>
+      <c r="D58" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E58" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="45">
       <c r="A59" s="5" t="s">
-        <v>190</v>
+        <v>172</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>191</v>
+        <v>173</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>192</v>
-      </c>
-      <c r="D59" s="6">
-        <v>12</v>
-      </c>
-      <c r="E59" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="45">
-      <c r="A60" s="5" t="s">
-        <v>193</v>
+        <v>174</v>
+      </c>
+      <c r="D59" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E59" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="30">
+      <c r="A60" t="s">
+        <v>384</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>194</v>
+        <v>385</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>195</v>
-      </c>
-      <c r="D60" s="6">
-        <v>5</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" ht="60">
+        <v>386</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="6" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="45">
       <c r="A61" s="5" t="s">
-        <v>196</v>
+        <v>434</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>197</v>
+        <v>435</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D61" s="6">
-        <v>13</v>
-      </c>
-      <c r="E61" s="7" t="s">
-        <v>12</v>
+        <v>436</v>
+      </c>
+      <c r="D61" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="6" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="30">
       <c r="A62" s="5" t="s">
-        <v>199</v>
+        <v>28</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>200</v>
+        <v>29</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>201</v>
+        <v>30</v>
       </c>
       <c r="D62" s="6">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E62" s="7" t="s">
         <v>31</v>
@@ -4074,254 +4234,254 @@
     </row>
     <row r="63" spans="1:5" ht="45">
       <c r="A63" s="5" t="s">
-        <v>202</v>
+        <v>42</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>203</v>
+        <v>43</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="D63" s="6" t="s">
-        <v>8</v>
+        <v>44</v>
+      </c>
+      <c r="D63" s="6">
+        <v>2</v>
       </c>
       <c r="E63" s="7" t="s">
-        <v>205</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="30">
       <c r="A64" s="5" t="s">
-        <v>206</v>
+        <v>45</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>207</v>
+        <v>46</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>208</v>
+        <v>47</v>
       </c>
       <c r="D64" s="6">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E64" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="60">
+    <row r="65" spans="1:5" ht="30">
       <c r="A65" s="5" t="s">
-        <v>209</v>
+        <v>54</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>210</v>
+        <v>55</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>211</v>
+        <v>56</v>
       </c>
       <c r="D65" s="6">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E65" s="7" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="66" spans="1:5" ht="30">
+    <row r="66" spans="1:5" ht="45">
       <c r="A66" s="5" t="s">
-        <v>212</v>
+        <v>71</v>
       </c>
       <c r="B66" s="3" t="s">
-        <v>213</v>
+        <v>72</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>214</v>
+        <v>73</v>
       </c>
       <c r="D66" s="6">
+        <v>5</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="60">
+      <c r="A67" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D67" s="6">
+        <v>6</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="30">
+      <c r="A68" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D68" s="6">
         <v>7</v>
       </c>
-      <c r="E66" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" ht="45">
-      <c r="A67" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>216</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="D67" s="6">
-        <v>14</v>
-      </c>
-      <c r="E67" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" ht="45">
-      <c r="A68" t="s">
-        <v>218</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>219</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>220</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>27</v>
+      <c r="E68" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="69" spans="1:5" ht="30">
       <c r="A69" s="5" t="s">
-        <v>221</v>
+        <v>111</v>
       </c>
       <c r="B69" s="3" t="s">
-        <v>222</v>
+        <v>112</v>
       </c>
       <c r="C69" s="3" t="s">
-        <v>223</v>
-      </c>
-      <c r="D69" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E69" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D69" s="6">
+        <v>8</v>
+      </c>
+      <c r="E69" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:5" ht="30">
       <c r="A70" s="5" t="s">
-        <v>224</v>
+        <v>147</v>
       </c>
       <c r="B70" s="3" t="s">
-        <v>225</v>
+        <v>148</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>8</v>
+        <v>149</v>
+      </c>
+      <c r="D70" s="6">
+        <v>9</v>
       </c>
       <c r="E70" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" ht="45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="30">
       <c r="A71" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="B71" s="3" t="s">
-        <v>228</v>
+        <v>198</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>531</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>229</v>
+        <v>199</v>
       </c>
       <c r="D71" s="6">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E71" s="7" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="72" spans="1:5" ht="30">
       <c r="A72" s="5" t="s">
-        <v>230</v>
+        <v>204</v>
       </c>
       <c r="B72" s="3" t="s">
-        <v>231</v>
+        <v>205</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="D72" s="6" t="s">
-        <v>8</v>
+        <v>206</v>
+      </c>
+      <c r="D72" s="6">
+        <v>11</v>
       </c>
       <c r="E72" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="60">
       <c r="A73" s="5" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>233</v>
+        <v>208</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="D73" s="6">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E73" s="7" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
     </row>
     <row r="74" spans="1:5" ht="30">
       <c r="A74" s="5" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>8</v>
+        <v>244</v>
+      </c>
+      <c r="D74" s="6">
+        <v>13</v>
       </c>
       <c r="E74" s="7" t="s">
-        <v>60</v>
+        <v>31</v>
       </c>
     </row>
     <row r="75" spans="1:5" ht="45">
       <c r="A75" s="5" t="s">
-        <v>238</v>
+        <v>272</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>239</v>
+        <v>273</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>240</v>
+        <v>274</v>
       </c>
       <c r="D75" s="6">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E75" s="7" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
     </row>
     <row r="76" spans="1:5" ht="30">
       <c r="A76" s="5" t="s">
-        <v>241</v>
+        <v>301</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>242</v>
+        <v>302</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="D76" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E76" s="8" t="s">
-        <v>19</v>
+        <v>303</v>
+      </c>
+      <c r="D76" s="6">
+        <v>15</v>
+      </c>
+      <c r="E76" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:5" ht="30">
       <c r="A77" s="5" t="s">
-        <v>244</v>
+        <v>318</v>
       </c>
       <c r="B77" s="3" t="s">
-        <v>245</v>
+        <v>319</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>246</v>
+        <v>320</v>
       </c>
       <c r="D77" s="6">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E77" s="7" t="s">
         <v>31</v>
@@ -4329,883 +4489,883 @@
     </row>
     <row r="78" spans="1:5" ht="30">
       <c r="A78" s="5" t="s">
-        <v>247</v>
+        <v>327</v>
       </c>
       <c r="B78" s="3" t="s">
-        <v>248</v>
+        <v>328</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>249</v>
-      </c>
-      <c r="D78" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E78" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5" ht="60">
+        <v>329</v>
+      </c>
+      <c r="D78" s="6">
+        <v>17</v>
+      </c>
+      <c r="E78" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" s="5" t="s">
-        <v>250</v>
+        <v>387</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>251</v>
+        <v>388</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="D79" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E79" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5" ht="45">
-      <c r="A80" s="5" t="s">
-        <v>253</v>
+        <v>389</v>
+      </c>
+      <c r="D79" s="6">
+        <v>18</v>
+      </c>
+      <c r="E79" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="60">
+      <c r="A80" t="s">
+        <v>404</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>254</v>
+        <v>405</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>8</v>
+        <v>406</v>
+      </c>
+      <c r="D80" s="6">
+        <v>19</v>
       </c>
       <c r="E80" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="81" spans="1:5" ht="45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="30">
       <c r="A81" s="5" t="s">
-        <v>256</v>
+        <v>423</v>
       </c>
       <c r="B81" s="3" t="s">
-        <v>257</v>
+        <v>424</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>27</v>
+        <v>425</v>
+      </c>
+      <c r="D81" s="6">
+        <v>20</v>
+      </c>
+      <c r="E81" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:5" ht="30">
       <c r="A82" s="5" t="s">
-        <v>259</v>
+        <v>437</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>260</v>
+        <v>438</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="D82" s="6" t="s">
-        <v>8</v>
+        <v>439</v>
+      </c>
+      <c r="D82" s="6">
+        <v>21</v>
       </c>
       <c r="E82" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" ht="45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" ht="30">
       <c r="A83" s="5" t="s">
-        <v>262</v>
+        <v>461</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>263</v>
+        <v>462</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>264</v>
+        <v>463</v>
       </c>
       <c r="D83" s="6">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E83" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="84" spans="1:5" ht="30">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" ht="45">
       <c r="A84" s="5" t="s">
-        <v>265</v>
+        <v>476</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>266</v>
+        <v>477</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>8</v>
+        <v>478</v>
+      </c>
+      <c r="D84" s="6">
+        <v>23</v>
       </c>
       <c r="E84" s="7" t="s">
-        <v>205</v>
+        <v>31</v>
       </c>
     </row>
     <row r="85" spans="1:5" ht="45">
-      <c r="A85" t="s">
-        <v>268</v>
-      </c>
-      <c r="B85" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="D85" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E85" s="8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" ht="60">
+      <c r="A85" s="5" t="s">
+        <v>491</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C85" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="D85" s="6">
+        <v>24</v>
+      </c>
+      <c r="E85" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" ht="30">
       <c r="A86" s="5" t="s">
-        <v>271</v>
+        <v>527</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>272</v>
+        <v>528</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>273</v>
+        <v>529</v>
       </c>
       <c r="D86" s="6">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E86" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" ht="45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" ht="30">
       <c r="A87" s="5" t="s">
-        <v>274</v>
+        <v>219</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>275</v>
+        <v>220</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>276</v>
-      </c>
-      <c r="D87" s="6">
-        <v>14</v>
-      </c>
-      <c r="E87" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="D87" s="7">
+        <v>26</v>
+      </c>
+      <c r="E87" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:5" ht="30">
+    <row r="88" spans="1:5" ht="60">
       <c r="A88" s="5" t="s">
-        <v>277</v>
+        <v>61</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>278</v>
+        <v>62</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>279</v>
-      </c>
-      <c r="D88" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E88" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="89" spans="1:5" ht="45">
+        <v>63</v>
+      </c>
+      <c r="D88" s="6">
+        <v>27</v>
+      </c>
+      <c r="E88" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" ht="30">
       <c r="A89" s="5" t="s">
-        <v>280</v>
+        <v>426</v>
       </c>
       <c r="B89" s="3" t="s">
-        <v>281</v>
+        <v>427</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="D89" s="6">
-        <v>10</v>
-      </c>
-      <c r="E89" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="90" spans="1:5" ht="45">
+        <v>428</v>
+      </c>
+      <c r="D89" s="7">
+        <v>28</v>
+      </c>
+      <c r="E89" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" s="5" t="s">
-        <v>283</v>
+        <v>345</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>284</v>
+        <v>346</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="D90" s="6">
-        <v>11</v>
-      </c>
-      <c r="E90" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" ht="60">
+        <v>347</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="E90" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" ht="45">
       <c r="A91" s="5" t="s">
-        <v>286</v>
+        <v>470</v>
       </c>
       <c r="B91" s="3" t="s">
-        <v>287</v>
+        <v>471</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>288</v>
+        <v>472</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E91" s="7" t="s">
-        <v>38</v>
+        <v>533</v>
+      </c>
+      <c r="E91" s="9" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="92" spans="1:5" ht="45">
       <c r="A92" s="5" t="s">
-        <v>286</v>
+        <v>236</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>289</v>
+        <v>237</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>290</v>
-      </c>
-      <c r="D92" s="6">
-        <v>7</v>
-      </c>
-      <c r="E92" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>534</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" ht="45">
+      <c r="A93" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C93" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="E93" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" ht="45">
+      <c r="A94" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C94" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D94" s="6">
+        <v>2</v>
+      </c>
+      <c r="E94" s="7" t="s">
         <v>64</v>
-      </c>
-    </row>
-    <row r="93" spans="1:5" ht="30">
-      <c r="A93" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="B93" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="D93" s="6">
-        <v>17</v>
-      </c>
-      <c r="E93" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" ht="30">
-      <c r="A94" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="B94" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="D94" s="6">
-        <v>18</v>
-      </c>
-      <c r="E94" s="7" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="95" spans="1:5" ht="60">
       <c r="A95" s="5" t="s">
-        <v>297</v>
+        <v>32</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>298</v>
+        <v>33</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E95" s="7" t="s">
-        <v>94</v>
+        <v>34</v>
+      </c>
+      <c r="D95" s="6">
+        <v>3</v>
+      </c>
+      <c r="E95" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="96" spans="1:5" ht="30">
       <c r="A96" s="5" t="s">
-        <v>300</v>
+        <v>172</v>
       </c>
       <c r="B96" s="3" t="s">
-        <v>301</v>
+        <v>175</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>302</v>
-      </c>
-      <c r="D96" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="D96" s="6">
+        <v>4</v>
+      </c>
+      <c r="E96" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="45">
+      <c r="A97" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C97" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D97" s="6">
+        <v>5</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" ht="30">
+      <c r="A98" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="C98" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="D98" s="6">
+        <v>6</v>
+      </c>
+      <c r="E98" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" ht="45">
+      <c r="A99" s="5" t="s">
+        <v>284</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C99" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D99" s="6">
+        <v>7</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="30">
+      <c r="A100" t="s">
+        <v>330</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C100" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="D100" s="6">
         <v>8</v>
       </c>
-      <c r="E96" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="97" spans="1:5" ht="30">
-      <c r="A97" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="B97" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="C97" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="D97" s="6">
-        <v>15</v>
-      </c>
-      <c r="E97" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="98" spans="1:5" ht="45">
-      <c r="A98" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="B98" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="C98" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E98" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" ht="30">
-      <c r="A99" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="B99" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="C99" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="D99" s="6">
-        <v>12</v>
-      </c>
-      <c r="E99" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" ht="45">
-      <c r="A100" s="5" t="s">
-        <v>311</v>
-      </c>
-      <c r="B100" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="C100" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="E100" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="101" spans="1:5" ht="30">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="45">
       <c r="A101" s="5" t="s">
-        <v>314</v>
+        <v>333</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>315</v>
+        <v>334</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>316</v>
+        <v>335</v>
       </c>
       <c r="D101" s="6">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="E101" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="102" spans="1:5" ht="30">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" ht="45">
       <c r="A102" s="5" t="s">
-        <v>317</v>
+        <v>348</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>318</v>
+        <v>349</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>319</v>
+        <v>350</v>
       </c>
       <c r="D102" s="6">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="E102" s="7" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="103" spans="1:5" ht="30">
       <c r="A103" s="5" t="s">
-        <v>320</v>
+        <v>363</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>321</v>
+        <v>364</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>322</v>
+        <v>365</v>
       </c>
       <c r="D103" s="6">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E103" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="30">
-      <c r="A104" t="s">
-        <v>323</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="45">
+      <c r="A104" s="5" t="s">
+        <v>410</v>
       </c>
       <c r="B104" s="3" t="s">
-        <v>324</v>
+        <v>411</v>
       </c>
       <c r="C104" s="3" t="s">
-        <v>325</v>
+        <v>412</v>
       </c>
       <c r="D104" s="6">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E104" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="105" spans="1:5" ht="45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="30">
       <c r="A105" s="5" t="s">
-        <v>326</v>
+        <v>413</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>327</v>
+        <v>414</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>8</v>
+        <v>415</v>
+      </c>
+      <c r="D105" s="6">
+        <v>14</v>
       </c>
       <c r="E105" s="7" t="s">
-        <v>130</v>
+        <v>64</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="30">
       <c r="A106" s="5" t="s">
-        <v>329</v>
+        <v>416</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>330</v>
+        <v>417</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>331</v>
+        <v>418</v>
       </c>
       <c r="D106" s="6">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E106" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="107" spans="1:5" ht="30">
-      <c r="A107" t="s">
-        <v>332</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" ht="75">
+      <c r="A107" s="5" t="s">
+        <v>446</v>
       </c>
       <c r="B107" s="3" t="s">
-        <v>333</v>
+        <v>447</v>
       </c>
       <c r="C107" s="3" t="s">
-        <v>334</v>
+        <v>448</v>
       </c>
       <c r="D107" s="6">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E107" s="7" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="45">
-      <c r="A108" s="5" t="s">
-        <v>335</v>
+      <c r="A108" t="s">
+        <v>452</v>
       </c>
       <c r="B108" s="3" t="s">
-        <v>336</v>
+        <v>453</v>
       </c>
       <c r="C108" s="3" t="s">
-        <v>337</v>
+        <v>454</v>
       </c>
       <c r="D108" s="6">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="E108" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="109" spans="1:5" ht="60">
+    <row r="109" spans="1:5" ht="75">
       <c r="A109" s="5" t="s">
-        <v>338</v>
+        <v>464</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>339</v>
+        <v>465</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>340</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>8</v>
+        <v>466</v>
+      </c>
+      <c r="D109" s="6">
+        <v>18</v>
       </c>
       <c r="E109" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" ht="45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="30">
       <c r="A110" s="5" t="s">
-        <v>341</v>
+        <v>482</v>
       </c>
       <c r="B110" s="3" t="s">
-        <v>342</v>
+        <v>483</v>
       </c>
       <c r="C110" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>8</v>
+        <v>484</v>
+      </c>
+      <c r="D110" s="6">
+        <v>19</v>
       </c>
       <c r="E110" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" ht="75">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" ht="45">
       <c r="A111" s="5" t="s">
-        <v>344</v>
+        <v>488</v>
       </c>
       <c r="B111" s="3" t="s">
-        <v>345</v>
+        <v>489</v>
       </c>
       <c r="C111" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>8</v>
+        <v>490</v>
+      </c>
+      <c r="D111" s="6">
+        <v>20</v>
       </c>
       <c r="E111" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5">
-      <c r="A112" s="5" t="s">
-        <v>347</v>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="30">
+      <c r="A112" t="s">
+        <v>491</v>
       </c>
       <c r="B112" s="3" t="s">
-        <v>348</v>
+        <v>494</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="D112" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E112" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="113" spans="1:5" ht="45">
+        <v>495</v>
+      </c>
+      <c r="D112" s="6">
+        <v>21</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" ht="30">
       <c r="A113" s="5" t="s">
-        <v>350</v>
+        <v>491</v>
       </c>
       <c r="B113" s="3" t="s">
-        <v>351</v>
+        <v>496</v>
       </c>
       <c r="C113" s="3" t="s">
-        <v>352</v>
+        <v>497</v>
       </c>
       <c r="D113" s="6">
-        <v>10</v>
+        <v>22</v>
       </c>
       <c r="E113" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="114" spans="1:5" ht="30">
+    <row r="114" spans="1:5" ht="45">
       <c r="A114" s="5" t="s">
-        <v>353</v>
+        <v>521</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>354</v>
+        <v>522</v>
       </c>
       <c r="C114" s="3" t="s">
-        <v>355</v>
+        <v>523</v>
       </c>
       <c r="D114" s="6">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="E114" s="7" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="115" spans="1:5" ht="60">
+    <row r="115" spans="1:5" ht="30">
       <c r="A115" s="5" t="s">
-        <v>356</v>
+        <v>222</v>
       </c>
       <c r="B115" s="3" t="s">
-        <v>357</v>
+        <v>223</v>
       </c>
       <c r="C115" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="D115" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E115" s="7" t="s">
-        <v>134</v>
+        <v>224</v>
+      </c>
+      <c r="D115" s="6">
+        <v>25</v>
+      </c>
+      <c r="E115" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="116" spans="1:5" ht="30">
       <c r="A116" s="5" t="s">
-        <v>359</v>
+        <v>473</v>
       </c>
       <c r="B116" s="3" t="s">
-        <v>360</v>
+        <v>474</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>361</v>
+        <v>475</v>
       </c>
       <c r="D116" s="6">
-        <v>21</v>
-      </c>
-      <c r="E116" s="7" t="s">
-        <v>12</v>
+        <v>26</v>
+      </c>
+      <c r="E116" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="117" spans="1:5" ht="30">
       <c r="A117" s="5" t="s">
-        <v>362</v>
+        <v>180</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>363</v>
+        <v>181</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>364</v>
-      </c>
-      <c r="D117" s="7" t="s">
-        <v>98</v>
+        <v>182</v>
+      </c>
+      <c r="D117" s="6">
+        <v>27</v>
       </c>
       <c r="E117" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="118" spans="1:5" ht="30">
+    <row r="118" spans="1:5">
       <c r="A118" s="5" t="s">
-        <v>365</v>
+        <v>141</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>366</v>
+        <v>537</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>367</v>
+        <v>536</v>
       </c>
       <c r="D118" s="6">
-        <v>12</v>
-      </c>
-      <c r="E118" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E118" s="8" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="45">
+    <row r="119" spans="1:5" ht="30">
       <c r="A119" s="5" t="s">
-        <v>368</v>
+        <v>95</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>369</v>
+        <v>96</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>370</v>
+        <v>97</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E119" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" ht="45">
+        <v>532</v>
+      </c>
+      <c r="E119" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="120" spans="1:5" ht="30">
       <c r="A120" s="5" t="s">
-        <v>371</v>
+        <v>360</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>372</v>
+        <v>361</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="D120" s="6">
-        <v>14</v>
-      </c>
-      <c r="E120" s="7" t="s">
-        <v>19</v>
+        <v>362</v>
+      </c>
+      <c r="D120" s="6" t="s">
+        <v>533</v>
+      </c>
+      <c r="E120" s="8" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="121" spans="1:5" ht="30">
       <c r="A121" s="5" t="s">
-        <v>374</v>
+        <v>245</v>
       </c>
       <c r="B121" s="3" t="s">
-        <v>375</v>
+        <v>246</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>376</v>
-      </c>
-      <c r="D121" s="7" t="s">
-        <v>98</v>
+        <v>247</v>
+      </c>
+      <c r="D121" s="6" t="s">
+        <v>534</v>
       </c>
       <c r="E121" s="8" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
     </row>
     <row r="122" spans="1:5" ht="30">
       <c r="A122" s="5" t="s">
-        <v>377</v>
+        <v>351</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>378</v>
+        <v>352</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>379</v>
-      </c>
-      <c r="D122" s="6">
-        <v>15</v>
-      </c>
-      <c r="E122" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="D122" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="E122" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="123" spans="1:5" ht="45">
+      <c r="A123" t="s">
+        <v>13</v>
+      </c>
+      <c r="B123" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C123" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D123" s="6">
+        <v>1</v>
+      </c>
+      <c r="E123" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="30">
-      <c r="A123" s="5" t="s">
-        <v>380</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>381</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>382</v>
-      </c>
-      <c r="D123" s="6">
-        <v>22</v>
-      </c>
-      <c r="E123" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" ht="60">
+    <row r="124" spans="1:5" ht="45">
       <c r="A124" s="5" t="s">
-        <v>383</v>
+        <v>86</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>384</v>
+        <v>89</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>385</v>
+        <v>90</v>
       </c>
       <c r="D124" s="6">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E124" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="125" spans="1:5" ht="30">
-      <c r="A125" t="s">
-        <v>386</v>
+    <row r="125" spans="1:5" ht="45">
+      <c r="A125" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>387</v>
+        <v>115</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="D125" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E125" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="D125" s="6">
+        <v>4</v>
+      </c>
+      <c r="E125" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="45">
+      <c r="A126" s="5" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="126" spans="1:5">
-      <c r="A126" s="5" t="s">
-        <v>389</v>
-      </c>
       <c r="B126" s="3" t="s">
-        <v>390</v>
+        <v>155</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>391</v>
+        <v>156</v>
       </c>
       <c r="D126" s="6">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E126" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" ht="30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="127" spans="1:5" ht="45">
       <c r="A127" s="5" t="s">
-        <v>392</v>
+        <v>169</v>
       </c>
       <c r="B127" s="3" t="s">
-        <v>393</v>
+        <v>170</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>394</v>
+        <v>171</v>
       </c>
       <c r="D127" s="6">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="E127" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="128" spans="1:5" ht="60">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5" ht="30">
       <c r="A128" s="5" t="s">
-        <v>395</v>
+        <v>210</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>396</v>
+        <v>211</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>397</v>
+        <v>212</v>
       </c>
       <c r="D128" s="6">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E128" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="129" spans="1:5" ht="45">
+    <row r="129" spans="1:5" ht="60">
       <c r="A129" s="5" t="s">
-        <v>395</v>
+        <v>269</v>
       </c>
       <c r="B129" s="3" t="s">
-        <v>398</v>
+        <v>270</v>
       </c>
       <c r="C129" s="3" t="s">
-        <v>399</v>
+        <v>271</v>
       </c>
       <c r="D129" s="6">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="E129" s="7" t="s">
         <v>19</v>
@@ -5213,764 +5373,764 @@
     </row>
     <row r="130" spans="1:5" ht="45">
       <c r="A130" s="5" t="s">
-        <v>400</v>
+        <v>278</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>401</v>
+        <v>279</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D130" s="6" t="s">
-        <v>8</v>
+        <v>280</v>
+      </c>
+      <c r="D130" s="6">
+        <v>10</v>
       </c>
       <c r="E130" s="7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="131" spans="1:5" ht="45">
       <c r="A131" s="5" t="s">
-        <v>403</v>
+        <v>281</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>404</v>
+        <v>282</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>405</v>
+        <v>283</v>
       </c>
       <c r="D131" s="6">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="E131" s="7" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="132" spans="1:5" ht="60">
-      <c r="A132" t="s">
-        <v>406</v>
+    <row r="132" spans="1:5" ht="30">
+      <c r="A132" s="5" t="s">
+        <v>304</v>
       </c>
       <c r="B132" s="3" t="s">
-        <v>407</v>
+        <v>307</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>408</v>
+        <v>308</v>
       </c>
       <c r="D132" s="6">
+        <v>12</v>
+      </c>
+      <c r="E132" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E132" s="7" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="133" spans="1:5" ht="30">
-      <c r="A133" t="s">
-        <v>409</v>
-      </c>
-      <c r="B133" s="4" t="s">
-        <v>410</v>
-      </c>
-      <c r="C133" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="D133" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E133" s="8" t="s">
+      <c r="A133" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="D133" s="6">
+        <v>13</v>
+      </c>
+      <c r="E133" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="134" spans="1:5" ht="45">
       <c r="A134" s="5" t="s">
-        <v>412</v>
+        <v>369</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>413</v>
+        <v>370</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>414</v>
+        <v>371</v>
       </c>
       <c r="D134" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E134" s="7" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
     </row>
     <row r="135" spans="1:5" ht="30">
       <c r="A135" s="5" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>416</v>
+        <v>376</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>417</v>
+        <v>377</v>
       </c>
       <c r="D135" s="6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E135" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="136" spans="1:5" ht="30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="136" spans="1:5" ht="60">
       <c r="A136" s="5" t="s">
-        <v>418</v>
+        <v>381</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>419</v>
+        <v>382</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>420</v>
+        <v>383</v>
       </c>
       <c r="D136" s="6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E136" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" ht="30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="60">
       <c r="A137" s="5" t="s">
-        <v>421</v>
+        <v>393</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>422</v>
+        <v>394</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>423</v>
-      </c>
-      <c r="D137" s="6" t="s">
-        <v>8</v>
+        <v>395</v>
+      </c>
+      <c r="D137" s="6">
+        <v>17</v>
       </c>
       <c r="E137" s="7" t="s">
-        <v>424</v>
+        <v>19</v>
       </c>
     </row>
     <row r="138" spans="1:5" ht="45">
       <c r="A138" s="5" t="s">
-        <v>425</v>
+        <v>393</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>426</v>
+        <v>396</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>427</v>
-      </c>
-      <c r="D138" s="6" t="s">
-        <v>8</v>
+        <v>397</v>
+      </c>
+      <c r="D138" s="6">
+        <v>18</v>
       </c>
       <c r="E138" s="7" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="139" spans="1:5" ht="30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" ht="45">
       <c r="A139" s="5" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
       <c r="B139" s="3" t="s">
-        <v>429</v>
+        <v>402</v>
       </c>
       <c r="C139" s="3" t="s">
-        <v>430</v>
+        <v>403</v>
       </c>
       <c r="D139" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E139" s="7" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
     </row>
     <row r="140" spans="1:5" ht="30">
       <c r="A140" s="5" t="s">
-        <v>431</v>
+        <v>491</v>
       </c>
       <c r="B140" s="3" t="s">
-        <v>432</v>
+        <v>498</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>433</v>
-      </c>
-      <c r="D140" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E140" s="8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" ht="30">
+        <v>499</v>
+      </c>
+      <c r="D140" s="6">
+        <v>20</v>
+      </c>
+      <c r="E140" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="141" spans="1:5" ht="45">
       <c r="A141" s="5" t="s">
-        <v>431</v>
+        <v>506</v>
       </c>
       <c r="B141" s="3" t="s">
-        <v>434</v>
+        <v>507</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>435</v>
-      </c>
-      <c r="D141" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E141" s="8" t="s">
-        <v>12</v>
+        <v>508</v>
+      </c>
+      <c r="D141" s="6">
+        <v>21</v>
+      </c>
+      <c r="E141" s="7" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="142" spans="1:5" ht="30">
       <c r="A142" s="5" t="s">
-        <v>436</v>
+        <v>509</v>
       </c>
       <c r="B142" s="3" t="s">
-        <v>437</v>
+        <v>510</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>438</v>
+        <v>511</v>
       </c>
       <c r="D142" s="6">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E142" s="7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" ht="45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" ht="30">
       <c r="A143" s="5" t="s">
-        <v>439</v>
+        <v>292</v>
       </c>
       <c r="B143" s="3" t="s">
-        <v>440</v>
+        <v>293</v>
       </c>
       <c r="C143" s="3" t="s">
-        <v>441</v>
-      </c>
-      <c r="D143" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E143" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" ht="30">
+        <v>294</v>
+      </c>
+      <c r="D143" s="6">
+        <v>23</v>
+      </c>
+      <c r="E143" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="144" spans="1:5" ht="45">
       <c r="A144" s="5" t="s">
-        <v>442</v>
+        <v>500</v>
       </c>
       <c r="B144" s="3" t="s">
-        <v>443</v>
+        <v>501</v>
       </c>
       <c r="C144" s="3" t="s">
-        <v>444</v>
-      </c>
-      <c r="D144" s="6">
-        <v>21</v>
-      </c>
-      <c r="E144" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="145" spans="1:5" ht="60">
-      <c r="A145" s="5" t="s">
-        <v>445</v>
-      </c>
-      <c r="B145" s="3" t="s">
-        <v>446</v>
-      </c>
-      <c r="C145" s="3" t="s">
-        <v>447</v>
+        <v>502</v>
+      </c>
+      <c r="D144" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="E144" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5" ht="45">
+      <c r="A145" t="s">
+        <v>120</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C145" s="4" t="s">
+        <v>122</v>
       </c>
       <c r="D145" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E145" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="146" spans="1:5" ht="45">
+        <v>533</v>
+      </c>
+      <c r="E145" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5" ht="30">
       <c r="A146" s="5" t="s">
-        <v>448</v>
+        <v>239</v>
       </c>
       <c r="B146" s="3" t="s">
-        <v>449</v>
+        <v>240</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>450</v>
+        <v>241</v>
       </c>
       <c r="D146" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E146" s="7" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="147" spans="1:5" ht="75">
+        <v>534</v>
+      </c>
+      <c r="E146" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" ht="30">
       <c r="A147" s="5" t="s">
-        <v>451</v>
+        <v>372</v>
       </c>
       <c r="B147" s="3" t="s">
-        <v>452</v>
+        <v>373</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>453</v>
-      </c>
-      <c r="D147" s="6">
-        <v>16</v>
-      </c>
-      <c r="E147" s="7" t="s">
-        <v>64</v>
+        <v>374</v>
+      </c>
+      <c r="D147" s="6" t="s">
+        <v>535</v>
+      </c>
+      <c r="E147" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="148" spans="1:5" ht="45">
       <c r="A148" s="5" t="s">
-        <v>454</v>
+        <v>5</v>
       </c>
       <c r="B148" s="3" t="s">
-        <v>455</v>
+        <v>10</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>456</v>
-      </c>
-      <c r="D148" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E148" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D148" s="6">
+        <v>1</v>
+      </c>
+      <c r="E148" s="7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="149" spans="1:5" ht="45">
-      <c r="A149" t="s">
-        <v>457</v>
+    <row r="149" spans="1:5" ht="30">
+      <c r="A149" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="B149" s="3" t="s">
-        <v>458</v>
+        <v>69</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>459</v>
+        <v>70</v>
       </c>
       <c r="D149" s="6">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="E149" s="7" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="150" spans="1:5" ht="30">
       <c r="A150" s="5" t="s">
-        <v>460</v>
+        <v>102</v>
       </c>
       <c r="B150" s="3" t="s">
-        <v>461</v>
+        <v>103</v>
       </c>
       <c r="C150" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="D150" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D150" s="6">
+        <v>4</v>
+      </c>
+      <c r="E150" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" ht="45">
+      <c r="A151" t="s">
+        <v>105</v>
+      </c>
+      <c r="B151" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D151" s="6">
+        <v>5</v>
+      </c>
+      <c r="E151" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" ht="30">
+      <c r="A152" t="s">
+        <v>117</v>
+      </c>
+      <c r="B152" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D152" s="6">
+        <v>6</v>
+      </c>
+      <c r="E152" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" ht="45">
+      <c r="A153" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="D153" s="6">
+        <v>7</v>
+      </c>
+      <c r="E153" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" ht="60">
+      <c r="A154" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D154" s="6">
         <v>8</v>
       </c>
-      <c r="E150" s="7" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="151" spans="1:5" ht="45">
-      <c r="A151" s="5" t="s">
-        <v>463</v>
-      </c>
-      <c r="B151" s="3" t="s">
-        <v>464</v>
-      </c>
-      <c r="C151" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="D151" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E151" s="7" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="152" spans="1:5" ht="30">
-      <c r="A152" s="5" t="s">
-        <v>466</v>
-      </c>
-      <c r="B152" s="3" t="s">
-        <v>467</v>
-      </c>
-      <c r="C152" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="D152" s="6">
-        <v>22</v>
-      </c>
-      <c r="E152" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="153" spans="1:5" ht="75">
-      <c r="A153" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="B153" s="3" t="s">
-        <v>470</v>
-      </c>
-      <c r="C153" s="3" t="s">
-        <v>471</v>
-      </c>
-      <c r="D153" s="6">
-        <v>18</v>
-      </c>
-      <c r="E153" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="154" spans="1:5" ht="30">
-      <c r="A154" s="5" t="s">
-        <v>472</v>
-      </c>
-      <c r="B154" s="3" t="s">
-        <v>473</v>
-      </c>
-      <c r="C154" s="3" t="s">
-        <v>474</v>
-      </c>
-      <c r="D154" s="6" t="s">
-        <v>8</v>
-      </c>
       <c r="E154" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="155" spans="1:5" ht="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" ht="30">
       <c r="A155" s="5" t="s">
-        <v>475</v>
+        <v>166</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>476</v>
+        <v>167</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>477</v>
-      </c>
-      <c r="D155" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E155" s="9" t="s">
-        <v>31</v>
+        <v>168</v>
+      </c>
+      <c r="D155" s="6">
+        <v>10</v>
+      </c>
+      <c r="E155" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="156" spans="1:5" ht="30">
       <c r="A156" s="5" t="s">
-        <v>478</v>
+        <v>186</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>479</v>
+        <v>187</v>
       </c>
       <c r="C156" s="3" t="s">
-        <v>480</v>
-      </c>
-      <c r="D156" s="6" t="s">
-        <v>8</v>
+        <v>188</v>
+      </c>
+      <c r="D156" s="6">
+        <v>11</v>
       </c>
       <c r="E156" s="7" t="s">
-        <v>424</v>
-      </c>
-    </row>
-    <row r="157" spans="1:5" ht="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5" ht="30">
       <c r="A157" s="5" t="s">
-        <v>481</v>
+        <v>189</v>
       </c>
       <c r="B157" s="3" t="s">
-        <v>482</v>
+        <v>190</v>
       </c>
       <c r="C157" s="3" t="s">
-        <v>483</v>
+        <v>191</v>
       </c>
       <c r="D157" s="6">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="E157" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="158" spans="1:5" ht="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="158" spans="1:5" ht="60">
       <c r="A158" s="5" t="s">
-        <v>484</v>
+        <v>195</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>485</v>
+        <v>196</v>
       </c>
       <c r="C158" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="D158" s="6" t="s">
-        <v>8</v>
+        <v>197</v>
+      </c>
+      <c r="D158" s="6">
+        <v>13</v>
       </c>
       <c r="E158" s="7" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="159" spans="1:5" ht="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5" ht="45">
       <c r="A159" s="5" t="s">
-        <v>487</v>
+        <v>213</v>
       </c>
       <c r="B159" s="3" t="s">
-        <v>488</v>
+        <v>214</v>
       </c>
       <c r="C159" s="3" t="s">
-        <v>489</v>
+        <v>215</v>
       </c>
       <c r="D159" s="6">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E159" s="7" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="160" spans="1:5" ht="45">
       <c r="A160" s="5" t="s">
-        <v>490</v>
+        <v>225</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>491</v>
+        <v>226</v>
       </c>
       <c r="C160" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="D160" s="6" t="s">
-        <v>8</v>
+        <v>227</v>
+      </c>
+      <c r="D160" s="6">
+        <v>15</v>
       </c>
       <c r="E160" s="7" t="s">
-        <v>424</v>
+        <v>12</v>
       </c>
     </row>
     <row r="161" spans="1:5" ht="45">
       <c r="A161" s="5" t="s">
-        <v>493</v>
+        <v>260</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>494</v>
+        <v>261</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>495</v>
+        <v>262</v>
       </c>
       <c r="D161" s="6">
+        <v>16</v>
+      </c>
+      <c r="E161" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="162" spans="1:5" ht="30">
+      <c r="A162" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="D162" s="6">
+        <v>17</v>
+      </c>
+      <c r="E162" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="163" spans="1:5" ht="30">
+      <c r="A163" s="5" t="s">
+        <v>312</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="D163" s="6">
+        <v>19</v>
+      </c>
+      <c r="E163" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" ht="30">
+      <c r="A164" t="s">
+        <v>321</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="D164" s="6">
         <v>20</v>
       </c>
-      <c r="E161" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" ht="45">
-      <c r="A162" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="B162" s="3" t="s">
-        <v>497</v>
-      </c>
-      <c r="C162" s="3" t="s">
-        <v>498</v>
-      </c>
-      <c r="D162" s="6">
-        <v>24</v>
-      </c>
-      <c r="E162" s="7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" ht="30">
-      <c r="A163" t="s">
-        <v>496</v>
-      </c>
-      <c r="B163" s="3" t="s">
-        <v>499</v>
-      </c>
-      <c r="C163" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="D163" s="6">
-        <v>21</v>
-      </c>
-      <c r="E163" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" ht="30">
-      <c r="A164" s="5" t="s">
-        <v>496</v>
-      </c>
-      <c r="B164" s="3" t="s">
-        <v>501</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>502</v>
-      </c>
-      <c r="D164" s="6">
-        <v>22</v>
-      </c>
       <c r="E164" s="7" t="s">
-        <v>64</v>
+        <v>12</v>
       </c>
     </row>
     <row r="165" spans="1:5" ht="30">
       <c r="A165" s="5" t="s">
-        <v>496</v>
+        <v>357</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>503</v>
+        <v>358</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>504</v>
+        <v>359</v>
       </c>
       <c r="D165" s="6">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E165" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" ht="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" ht="30">
       <c r="A166" s="5" t="s">
-        <v>505</v>
+        <v>378</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>506</v>
+        <v>379</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="D166" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="E166" s="8" t="s">
-        <v>19</v>
+        <v>380</v>
+      </c>
+      <c r="D166" s="6">
+        <v>22</v>
+      </c>
+      <c r="E166" s="7" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="167" spans="1:5" ht="30">
       <c r="A167" s="5" t="s">
-        <v>508</v>
+        <v>390</v>
       </c>
       <c r="B167" s="3" t="s">
-        <v>509</v>
+        <v>391</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>510</v>
+        <v>392</v>
       </c>
       <c r="D167" s="6">
         <v>23</v>
       </c>
       <c r="E167" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" ht="45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" ht="30">
       <c r="A168" s="5" t="s">
-        <v>511</v>
+        <v>431</v>
       </c>
       <c r="B168" s="3" t="s">
-        <v>512</v>
+        <v>432</v>
       </c>
       <c r="C168" s="3" t="s">
-        <v>513</v>
+        <v>433</v>
       </c>
       <c r="D168" s="6">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E168" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" ht="30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" ht="60">
       <c r="A169" s="5" t="s">
-        <v>514</v>
+        <v>284</v>
       </c>
       <c r="B169" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="D169" s="6">
+        <v>25</v>
+      </c>
+      <c r="E169" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="170" spans="1:5" ht="60">
+      <c r="A170" s="5" t="s">
         <v>515</v>
       </c>
-      <c r="C169" s="3" t="s">
+      <c r="B170" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="D169" s="6">
-        <v>22</v>
-      </c>
-      <c r="E169" s="7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" ht="30">
-      <c r="A170" s="5" t="s">
+      <c r="C170" s="3" t="s">
         <v>517</v>
       </c>
-      <c r="B170" s="3" t="s">
-        <v>518</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>519</v>
-      </c>
-      <c r="D170" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E170" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" ht="60">
+      <c r="D170" s="6">
+        <v>26</v>
+      </c>
+      <c r="E170" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="171" spans="1:5" ht="30">
       <c r="A171" s="5" t="s">
-        <v>520</v>
+        <v>426</v>
       </c>
       <c r="B171" s="3" t="s">
-        <v>521</v>
+        <v>429</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="D171" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E171" s="7" t="s">
-        <v>424</v>
+        <v>430</v>
+      </c>
+      <c r="D171" s="7">
+        <v>27</v>
+      </c>
+      <c r="E171" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="172" spans="1:5" ht="45">
       <c r="A172" s="5" t="s">
-        <v>523</v>
+        <v>449</v>
       </c>
       <c r="B172" s="3" t="s">
-        <v>524</v>
+        <v>450</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>525</v>
-      </c>
-      <c r="D172" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E172" s="7" t="s">
-        <v>134</v>
+        <v>451</v>
+      </c>
+      <c r="D172" s="6">
+        <v>28</v>
+      </c>
+      <c r="E172" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="173" spans="1:5" ht="45">
       <c r="A173" s="5" t="s">
-        <v>526</v>
+        <v>157</v>
       </c>
       <c r="B173" s="3" t="s">
-        <v>527</v>
+        <v>158</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="D173" s="6">
-        <v>24</v>
-      </c>
-      <c r="E173" s="7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" ht="30">
-      <c r="A174" s="5" t="s">
-        <v>529</v>
-      </c>
-      <c r="B174" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="C174" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="D174" s="7" t="s">
-        <v>98</v>
+        <v>159</v>
+      </c>
+      <c r="D173" s="6" t="s">
+        <v>532</v>
+      </c>
+      <c r="E173" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="45">
+      <c r="A174" t="s">
+        <v>266</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="C174" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="D174" s="6" t="s">
+        <v>533</v>
       </c>
       <c r="E174" s="8" t="s">
         <v>12</v>
@@ -5978,27 +6138,36 @@
     </row>
     <row r="175" spans="1:5" ht="30">
       <c r="A175" s="5" t="s">
-        <v>532</v>
+        <v>524</v>
       </c>
       <c r="B175" s="3" t="s">
-        <v>533</v>
+        <v>525</v>
       </c>
       <c r="C175" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D175" s="6" t="s">
         <v>534</v>
       </c>
-      <c r="D175" s="6">
-        <v>25</v>
-      </c>
-      <c r="E175" s="7" t="s">
-        <v>31</v>
+      <c r="E175" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:I175">
+    <sortCondition ref="E2:E175"/>
+    <sortCondition ref="D2:D175"/>
+  </sortState>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
+  <pageSetup firstPageNumber="0" orientation="portrait"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>